<commit_message>
correct order of pokedex_entries.h parameters
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">evolves</t>
   </si>
   <si>
-    <t xml:space="preserve">EVO_LEVEL</t>
+    <t xml:space="preserve">EVO_FRIENDSHIP</t>
   </si>
   <si>
     <t xml:space="preserve">pokedex_entry_line1</t>
@@ -428,7 +428,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.48"/>
   </cols>
   <sheetData>
@@ -447,11 +447,11 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -459,69 +459,69 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="2" t="n">
         <f aca="false">LEN(B5)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
         <v>42</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -529,7 +529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -537,7 +537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -545,7 +545,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -553,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -561,7 +561,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -577,7 +577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -585,7 +585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -593,7 +593,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -601,7 +601,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -609,7 +609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
@@ -617,7 +617,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
@@ -625,7 +625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
@@ -633,7 +633,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
@@ -641,7 +641,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -649,7 +649,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -666,7 +666,7 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
@@ -706,7 +706,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>43</v>
       </c>
@@ -714,7 +714,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>45</v>
       </c>
@@ -722,7 +722,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
@@ -730,7 +730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>48</v>
       </c>
@@ -738,7 +738,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>49</v>
       </c>
@@ -746,7 +746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>51</v>
       </c>
@@ -802,18 +802,18 @@
       <c r="B43" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -824,7 +824,7 @@
       <c r="B45" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -835,7 +835,7 @@
       <c r="B46" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -846,7 +846,7 @@
       <c r="B47" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -854,15 +854,15 @@
       <c r="A48" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -870,15 +870,15 @@
       <c r="A50" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -886,7 +886,7 @@
       <c r="A52" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -894,7 +894,7 @@
       <c r="A53" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -902,7 +902,7 @@
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -910,7 +910,7 @@
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -918,71 +918,71 @@
       <c r="A56" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -990,15 +990,15 @@
       <c r="A65" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       <c r="A67" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1014,15 +1014,15 @@
       <c r="A68" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       <c r="A70" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       <c r="A71" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="2" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       <c r="A72" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="2" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trifox and Puddi display names
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="130">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -29,6 +29,12 @@
     <t xml:space="preserve">TRIFOX</t>
   </si>
   <si>
+    <t xml:space="preserve">display_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trifox</t>
+  </si>
+  <si>
     <t xml:space="preserve">where</t>
   </si>
   <si>
@@ -321,6 +327,9 @@
   </si>
   <si>
     <t xml:space="preserve">PUDDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puddi</t>
   </si>
   <si>
     <t xml:space="preserve">GROWLITHE</t>
@@ -592,10 +601,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -621,15 +630,15 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -638,13 +647,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,11 +655,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <f aca="false">LEN(B5)</f>
-        <v>40</v>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,7 +685,7 @@
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,80 +697,84 @@
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>30</v>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">LEN(B9)</f>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>256</v>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f aca="false">CONCATENATE("total: ",SUM(B15:B20))</f>
-        <v>total: 200</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f aca="false">CONCATENATE("total: ",SUM(B16:B21))</f>
+        <v>total: 200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>25</v>
@@ -773,34 +782,34 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,69 +817,69 @@
         <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>41</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>0</v>
@@ -878,10 +887,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,24 +913,24 @@
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="2" t="n">
-        <v>10</v>
+      <c r="B34" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="2" t="s">
         <v>50</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,15 +946,15 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,135 +977,135 @@
       <c r="A42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>28</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>74</v>
@@ -1104,63 +1113,63 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>81</v>
@@ -1168,71 +1177,71 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>91</v>
@@ -1240,62 +1249,70 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C8">
+  <conditionalFormatting sqref="C6:C9">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>44</formula>
     </cfRule>
@@ -1315,7 +1332,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1334,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,18 +1359,18 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>101</v>
+      <c r="C3" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,13 +1378,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,11 +1386,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <f aca="false">LEN(B5)</f>
-        <v>41</v>
+        <v>103</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1387,11 +1400,11 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,11 +1412,11 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,119 +1424,123 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>40</v>
+      <c r="B9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">LEN(B9)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>106</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>256</v>
+      <c r="B11" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f aca="false">CONCATENATE("total: ",SUM(B15:B20))</f>
-        <v>total: 200</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="n">
-        <v>40</v>
+      <c r="C16" s="2" t="str">
+        <f aca="false">CONCATENATE("total: ",SUM(B16:B21))</f>
+        <v>total: 200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,53 +1548,53 @@
         <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>41</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>0</v>
@@ -1585,7 +1602,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>0</v>
@@ -1593,7 +1610,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>0</v>
@@ -1601,10 +1618,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,7 +1629,7 @@
         <v>43</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,31 +1637,31 @@
         <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="2" t="n">
-        <v>10</v>
+      <c r="B34" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>108</v>
+        <v>50</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,7 +1669,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,15 +1677,15 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,7 +1693,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,277 +1701,277 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="2" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>30</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>91</v>
@@ -1962,70 +1979,78 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>126</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C8">
+  <conditionalFormatting sqref="C6:C9">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>44</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix Clone Charmander evo method
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="156">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -432,19 +432,16 @@
     <t xml:space="preserve">CHARMELEON</t>
   </si>
   <si>
-    <t xml:space="preserve">EVO_LEVEL_UP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
+    <t xml:space="preserve">EVO_LEVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An experimental species created by Dr. Fuji.</t>
   </si>
   <si>
     <t xml:space="preserve">9.2</t>
   </si>
   <si>
     <t xml:space="preserve">PERCENT_FEMALE(12.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROWTH_MEDIUM_SLOW</t>
   </si>
   <si>
     <t xml:space="preserve">EGG_GROUP_MONSTER</t>
@@ -1417,7 +1414,7 @@
   <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2154,8 +2151,8 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2224,7 +2221,7 @@
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,7 +2477,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,7 +2485,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,7 +2493,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,7 +2501,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,7 +2509,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2613,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2635,7 @@
         <v>28</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,7 +2646,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,7 +2657,7 @@
         <v>36</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2668,7 @@
         <v>40</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,7 +2676,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2687,7 +2684,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,7 +2692,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,7 +2716,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,7 +2724,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,7 +2732,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modify TM/HM move format in new_species excel
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="159">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -304,28 +304,25 @@
     <t xml:space="preserve">TM_MOVE</t>
   </si>
   <si>
-    <t xml:space="preserve">TM45 Attract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM27 Return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM32 Double Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM35 Flamethrower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM17 Protect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM05 Roar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM11 Sunny Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM06 Toxic</t>
+    <t xml:space="preserve">Attract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flamethrower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunny Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toxic</t>
   </si>
   <si>
     <t xml:space="preserve">PUDDI</t>
@@ -391,9 +388,6 @@
     <t xml:space="preserve">Retaliate</t>
   </si>
   <si>
-    <t xml:space="preserve">Flamethrower</t>
-  </si>
-  <si>
     <t xml:space="preserve">Covet</t>
   </si>
   <si>
@@ -412,7 +406,7 @@
     <t xml:space="preserve">Thunder Fang</t>
   </si>
   <si>
-    <t xml:space="preserve">TM46 Thief</t>
+    <t xml:space="preserve">Thief</t>
   </si>
   <si>
     <t xml:space="preserve">CLONE_CHARMANDER</t>
@@ -698,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C80" activeCellId="0" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1387,7 +1381,7 @@
         <v>92</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1395,7 +1389,7 @@
         <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,7 +1397,7 @@
         <v>92</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1429,8 +1423,8 @@
   </sheetPr>
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C81" activeCellId="0" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1446,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,7 +1459,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,7 +1467,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,7 +1475,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -1495,7 +1489,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -1507,7 +1501,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -1519,7 +1513,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -1531,7 +1525,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -1551,7 +1545,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1734,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,7 +1758,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,7 +1790,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,7 +1850,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,7 +1861,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1872,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,7 +1883,7 @@
         <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,7 +1894,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,7 +1905,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,7 +1916,7 @@
         <v>28</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1933,7 +1927,7 @@
         <v>30</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1941,7 +1935,7 @@
         <v>75</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1943,7 @@
         <v>75</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,7 +1951,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,7 +1967,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +1983,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,7 +1991,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2111,7 @@
         <v>92</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,7 +2119,7 @@
         <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2127,7 @@
         <v>92</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,7 +2135,7 @@
         <v>92</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2167,8 +2161,8 @@
   </sheetPr>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2184,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,7 +2186,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,10 +2194,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,7 +2205,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2219,10 +2213,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>16</v>
@@ -2233,7 +2227,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -2245,7 +2239,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -2257,7 +2251,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -2269,7 +2263,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -2289,7 +2283,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,7 +2472,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,7 +2504,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,7 +2512,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,7 +2520,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2534,7 +2528,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2599,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2610,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,7 +2621,7 @@
         <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2632,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,7 +2643,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,7 +2654,7 @@
         <v>28</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2665,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,7 +2676,7 @@
         <v>36</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2693,7 +2687,7 @@
         <v>40</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2701,7 +2695,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,7 +2703,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,7 +2711,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2725,7 +2719,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,7 +2727,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2741,7 +2735,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,7 +2743,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,7 +2751,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2863,7 @@
         <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2877,7 +2871,7 @@
         <v>92</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +2914,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2928,7 +2922,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2936,10 +2930,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,7 +2941,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2955,10 +2949,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>36</v>
@@ -3013,7 +3007,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3202,7 +3196,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3234,7 +3228,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,7 +3236,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3250,7 +3244,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,7 +3252,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,7 +3279,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3318,7 +3312,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,7 +3323,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3340,7 +3334,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,7 +3345,7 @@
         <v>19</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3362,7 +3356,7 @@
         <v>24</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3373,7 +3367,7 @@
         <v>30</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3384,7 +3378,7 @@
         <v>37</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3389,7 @@
         <v>42</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3406,7 +3400,7 @@
         <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,7 +3411,7 @@
         <v>56</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3425,7 +3419,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3433,7 +3427,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3441,7 +3435,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,7 +3443,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3457,7 +3451,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,7 +3459,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3473,7 +3467,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,7 +3475,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,7 +3587,7 @@
         <v>92</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3601,7 +3595,7 @@
         <v>92</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sort TM/HM moves automatically, work on Clone Charmander/Charmeleon
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="171">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -494,6 +494,42 @@
   </si>
   <si>
     <t xml:space="preserve">Mega Punch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon Claw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidden Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frustration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Tail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brick Break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secret Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock Smash</t>
   </si>
   <si>
     <t xml:space="preserve">CHARIZARD</t>
@@ -2159,10 +2195,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
+      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2872,6 +2908,102 @@
       </c>
       <c r="C79" s="2" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2895,10 +3027,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2949,7 +3081,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>134</v>
@@ -3007,7 +3139,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3596,6 +3728,102 @@
       </c>
       <c r="C79" s="2" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on Clone Charmeleon
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="175">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -533,6 +533,18 @@
   </si>
   <si>
     <t xml:space="preserve">CHARIZARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It has a harsh and volatile personality. In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange for its wicked physical attacks, it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has less good skills with fire. This POKéMON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is especially difficult to tame.</t>
   </si>
   <si>
     <t xml:space="preserve">26.4</t>
@@ -2197,8 +2209,8 @@
   </sheetPr>
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3029,8 +3041,8 @@
   </sheetPr>
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="0" sqref="A76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3065,7 +3077,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3094,36 +3106,48 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,7 +3163,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
work on Clone Bulbasaur
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Trifox" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Clone_Charmander" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Clone_Charmeleon" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Clone_Charizard" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Clone_Bulbasaur" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="228">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -588,6 +589,126 @@
   </si>
   <si>
     <t xml:space="preserve">Sacred Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLONE_BULBASAUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulbasaur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVYSAUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Fuji. It has a strong intuition and can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anticipate its enemy’s attacks. It will</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consider its strategy before moving.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE_GRASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPE_POISON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGG_GROUP_GRASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ABILITY_REGENERATOR,ABILITY_NONE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABILITY_REGENERATOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BODY_COLOR_GREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acid Spray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vine Whip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leech Seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aromatherapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf Tornado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synthesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poison Powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingrain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Ball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweet Scent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sludge Bomb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar Beam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nature Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petal Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Razor Leaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Whip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giga Drain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amnesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sludge Wave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defense Curl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fury Cutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mud Slap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swords Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bullet Seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flash</t>
   </si>
 </sst>
 </file>
@@ -3929,6 +4050,865 @@
   </sheetPr>
   <dimension ref="A1:G94"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.48"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">LEN(B5)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">LEN(B6)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">LEN(B7)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">LEN(B8)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f aca="false">CONCATENATE("total: ",SUM(B15:B20))</f>
+        <v>total: 540</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C5:C8">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>44</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normaali"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normaali"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G96"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -3946,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3954,7 +4934,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,7 +4945,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3978,34 +4958,36 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <f aca="false">LEN(B5)</f>
-        <v>40</v>
+        <v>190</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -4014,168 +4996,172 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>200</v>
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">LEN(B9)</f>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>182</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>256</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B15" s="2" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>94</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f aca="false">CONCATENATE("total: ",SUM(B15:B20))</f>
-        <v>total: 540</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>101</v>
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f aca="false">CONCATENATE("total: ",SUM(B16:B21))</f>
+        <v>total: 320</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>97</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>93</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>190</v>
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>41</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>0</v>
@@ -4183,7 +5169,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>0</v>
@@ -4191,7 +5177,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>0</v>
@@ -4199,23 +5185,23 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>46</v>
@@ -4223,93 +5209,90 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="2" t="n">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>143</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>61</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B43" s="2" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4320,7 +5303,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4331,7 +5314,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>66</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4339,10 +5322,10 @@
         <v>63</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4350,10 +5333,10 @@
         <v>63</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>115</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4361,10 +5344,10 @@
         <v>63</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4372,10 +5355,10 @@
         <v>63</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>118</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4383,10 +5366,10 @@
         <v>63</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,10 +5377,10 @@
         <v>63</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>119</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4405,10 +5388,10 @@
         <v>63</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4416,10 +5399,10 @@
         <v>63</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,10 +5410,10 @@
         <v>63</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4438,10 +5421,10 @@
         <v>63</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4449,10 +5432,10 @@
         <v>63</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>150</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4460,21 +5443,18 @@
         <v>63</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B58" s="2" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4482,7 +5462,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>151</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4490,7 +5470,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>152</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4498,7 +5478,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,7 +5486,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>126</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4514,7 +5494,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>124</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4522,7 +5502,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>154</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4530,7 +5510,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>155</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4538,7 +5518,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>156</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4546,7 +5526,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>157</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4562,7 +5542,7 @@
         <v>82</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>84</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4570,7 +5550,7 @@
         <v>82</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>85</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4578,7 +5558,7 @@
         <v>82</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>86</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4586,7 +5566,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4594,7 +5574,7 @@
         <v>82</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>88</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4602,7 +5582,7 @@
         <v>82</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4610,7 +5590,7 @@
         <v>82</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4618,28 +5598,28 @@
         <v>82</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>94</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>96</v>
@@ -4650,7 +5630,7 @@
         <v>92</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4658,7 +5638,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>98</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4666,7 +5646,7 @@
         <v>92</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4674,7 +5654,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4682,7 +5662,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>159</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4690,7 +5670,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>160</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4698,7 +5678,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4706,7 +5686,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4714,7 +5694,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>163</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4722,7 +5702,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4730,7 +5710,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4738,7 +5718,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4746,7 +5726,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4754,7 +5734,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4762,11 +5742,27 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C8">
+  <conditionalFormatting sqref="C6:C9">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>44</formula>
     </cfRule>

</xml_diff>

<commit_message>
Clone Ivysaur & Venusaur base stats
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Trifox" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,8 @@
     <sheet name="Clone_Charmeleon" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Clone_Charizard" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Clone_Bulbasaur" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Clone_Ivysaur" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Clone_Venusaur" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="245">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -591,22 +593,28 @@
     <t xml:space="preserve">Sacred Fire</t>
   </si>
   <si>
+    <t xml:space="preserve">Hyper Beam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Blast</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLONE_BULBASAUR</t>
   </si>
   <si>
     <t xml:space="preserve">Bulbasaur</t>
   </si>
   <si>
-    <t xml:space="preserve">IVYSAUR</t>
+    <t xml:space="preserve">CLONE_IVYSAUR</t>
   </si>
   <si>
     <t xml:space="preserve">Dr. Fuji. It has a strong intuition and can</t>
   </si>
   <si>
-    <t xml:space="preserve">anticipate its enemy’s attacks. It will</t>
-  </si>
-  <si>
-    <t xml:space="preserve">consider its strategy before moving.</t>
+    <t xml:space="preserve">anticipate its enemy’s attacks. It will plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">its strategy far ahead before moving.</t>
   </si>
   <si>
     <t xml:space="preserve">TYPE_GRASS</t>
@@ -654,7 +662,7 @@
     <t xml:space="preserve">Ingrain</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy Ball</t>
+    <t xml:space="preserve">Giga Drain</t>
   </si>
   <si>
     <t xml:space="preserve">Sweet Scent</t>
@@ -681,9 +689,6 @@
     <t xml:space="preserve">Spore</t>
   </si>
   <si>
-    <t xml:space="preserve">Giga Drain</t>
-  </si>
-  <si>
     <t xml:space="preserve">Amnesia</t>
   </si>
   <si>
@@ -709,6 +714,54 @@
   </si>
   <si>
     <t xml:space="preserve">Flash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivysaur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VENUSAUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It has a devious and cunning nature. It can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">easily predict its opponents tactic and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">react pre-emptively. The most insightful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intividuals surpass humans in intelligence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLONE_VENUSAUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venusaur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A masterful tactician, it can foresee the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events of a battle before it even starts. It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will make a surprising move and then deliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a single powerful blow to defeat the enemy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed Flare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earthquake</t>
   </si>
 </sst>
 </file>
@@ -3210,7 +3263,7 @@
   </sheetPr>
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4048,10 +4101,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C96" activeCellId="0" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4884,6 +4937,22 @@
       </c>
       <c r="C94" s="2" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4909,6 +4978,1756 @@
   </sheetPr>
   <dimension ref="A1:G96"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.48"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">LEN(B6)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">LEN(B7)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">LEN(B8)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">LEN(B9)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f aca="false">CONCATENATE("total: ",SUM(B16:B21))</f>
+        <v>total: 320</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C6:C9">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>44</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normaali"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normaali"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G96"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.48"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">LEN(B6)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">LEN(B7)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">LEN(B8)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">LEN(B9)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f aca="false">CONCATENATE("total: ",SUM(B16:B21))</f>
+        <v>total: 420</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C6:C9">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>44</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normaali"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normaali"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G101"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -4926,7 +6745,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4934,7 +6753,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>189</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,7 +6764,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>131</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4958,210 +6777,204 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>16</v>
+        <v>238</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">LEN(B5)</f>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>135</v>
+        <v>239</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <f aca="false">LEN(B9)</f>
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>75</v>
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>108</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>256</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
+      <c r="A15" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f aca="false">CONCATENATE("total: ",SUM(B15:B20))</f>
+        <v>total: 420</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f aca="false">CONCATENATE("total: ",SUM(B16:B21))</f>
-        <v>total: 320</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>195</v>
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>190</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>190</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>41</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>0</v>
@@ -5169,7 +6982,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>0</v>
@@ -5177,31 +6990,31 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>46</v>
@@ -5209,90 +7022,93 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>140</v>
+        <v>49</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="2" t="n">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>141</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>199</v>
+        <v>62</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
-        <v>62</v>
+      <c r="A43" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5303,7 +7119,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5314,7 +7130,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5322,10 +7138,10 @@
         <v>63</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5333,10 +7149,10 @@
         <v>63</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5344,10 +7160,10 @@
         <v>63</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5355,10 +7171,10 @@
         <v>63</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5366,10 +7182,10 @@
         <v>63</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5377,10 +7193,10 @@
         <v>63</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5388,10 +7204,10 @@
         <v>63</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5399,10 +7215,10 @@
         <v>63</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5410,10 +7226,10 @@
         <v>63</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5421,7 +7237,7 @@
         <v>63</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>99</v>
@@ -5432,10 +7248,10 @@
         <v>63</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5443,34 +7259,43 @@
         <v>63</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>60</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>65</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>70</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5478,7 +7303,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>99</v>
+        <v>210</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5502,7 +7327,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>217</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5510,7 +7335,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5518,7 +7343,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5526,31 +7351,31 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>83</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5558,7 +7383,7 @@
         <v>82</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>223</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5566,7 +7391,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>85</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5574,7 +7399,7 @@
         <v>82</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5582,7 +7407,7 @@
         <v>82</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5590,7 +7415,7 @@
         <v>82</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5598,7 +7423,7 @@
         <v>82</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>89</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5606,7 +7431,7 @@
         <v>82</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5614,7 +7439,7 @@
         <v>82</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>225</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5622,20 +7447,20 @@
         <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>226</v>
@@ -5643,10 +7468,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5654,7 +7479,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5662,7 +7487,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>97</v>
+        <v>227</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5670,7 +7495,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>218</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5678,7 +7503,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>160</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5686,7 +7511,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>212</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5694,7 +7519,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5702,7 +7527,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5710,7 +7535,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5718,7 +7543,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5726,7 +7551,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5734,7 +7559,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>93</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5742,7 +7567,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5750,7 +7575,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5758,11 +7583,51 @@
         <v>92</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>227</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C6:C9">
+  <conditionalFormatting sqref="C5:C8">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>44</formula>
     </cfRule>

</xml_diff>

<commit_message>
adjust height and weight
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Trifox" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="295">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t xml:space="preserve">a single powerful blow to defeat the enemy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">113.8</t>
   </si>
   <si>
     <t xml:space="preserve">Earth Power</t>
@@ -2571,8 +2574,8 @@
   </sheetPr>
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2685,7 +2688,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3446,7 +3449,7 @@
   </sheetPr>
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4321,7 +4324,7 @@
   </sheetPr>
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4421,7 +4424,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>110</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4429,7 +4432,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4866,7 +4869,7 @@
         <v>60</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4888,7 +4891,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5208,7 +5211,7 @@
         <v>92</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5216,7 +5219,7 @@
         <v>92</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -5259,7 +5262,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +5270,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5294,7 +5297,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>134</v>
@@ -5320,7 +5323,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -5332,7 +5335,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -5344,7 +5347,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -5364,7 +5367,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5593,7 +5596,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5601,7 +5604,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5609,7 +5612,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5617,7 +5620,7 @@
         <v>60</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5636,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5713,7 +5716,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5735,7 +5738,7 @@
         <v>28</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5746,7 +5749,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5757,7 +5760,7 @@
         <v>36</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5768,7 +5771,7 @@
         <v>40</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5776,7 +5779,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5784,7 +5787,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,7 +5795,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5816,7 +5819,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5824,7 +5827,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5832,7 +5835,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5840,7 +5843,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5968,7 +5971,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5992,7 +5995,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6000,7 +6003,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6008,7 +6011,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6016,7 +6019,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6056,7 +6059,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -6099,7 +6102,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6107,7 +6110,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6118,7 +6121,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6134,7 +6137,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>134</v>
@@ -6148,7 +6151,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -6160,7 +6163,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -6172,7 +6175,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -6184,7 +6187,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -6204,7 +6207,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6433,7 +6436,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6441,7 +6444,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6449,7 +6452,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6457,7 +6460,7 @@
         <v>60</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6476,7 +6479,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6553,7 +6556,7 @@
         <v>24</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6575,7 +6578,7 @@
         <v>37</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6586,7 +6589,7 @@
         <v>42</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6597,7 +6600,7 @@
         <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6608,7 +6611,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6616,7 +6619,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6624,7 +6627,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6632,7 +6635,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,7 +6659,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6664,7 +6667,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6672,7 +6675,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6680,7 +6683,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6808,7 +6811,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6832,7 +6835,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6840,7 +6843,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6848,7 +6851,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6856,7 +6859,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6896,7 +6899,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -6939,7 +6942,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6947,7 +6950,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6958,7 +6961,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6974,7 +6977,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C5" s="2" t="n">
         <f aca="false">LEN(B5)</f>
@@ -6986,7 +6989,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -6998,7 +7001,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -7010,7 +7013,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -7030,7 +7033,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7130,7 +7133,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7259,7 +7262,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7267,7 +7270,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7275,7 +7278,7 @@
         <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7283,7 +7286,7 @@
         <v>60</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7302,7 +7305,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7379,7 +7382,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7401,7 +7404,7 @@
         <v>36</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7412,7 +7415,7 @@
         <v>39</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7423,7 +7426,7 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7434,7 +7437,7 @@
         <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7445,7 +7448,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7456,7 +7459,7 @@
         <v>60</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7467,7 +7470,7 @@
         <v>65</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7478,7 +7481,7 @@
         <v>70</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7486,7 +7489,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7494,7 +7497,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7502,7 +7505,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7526,7 +7529,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7534,7 +7537,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7542,7 +7545,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7550,7 +7553,7 @@
         <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7558,7 +7561,7 @@
         <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7686,7 +7689,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7710,7 +7713,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7718,7 +7721,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7726,7 +7729,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7734,7 +7737,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7774,7 +7777,7 @@
         <v>92</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7782,7 +7785,7 @@
         <v>92</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7790,7 +7793,7 @@
         <v>92</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7798,7 +7801,7 @@
         <v>92</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -7824,8 +7827,8 @@
   </sheetPr>
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7841,7 +7844,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7849,7 +7852,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7860,7 +7863,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7876,7 +7879,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>134</v>
@@ -7902,7 +7905,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -7914,7 +7917,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -7926,7 +7929,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -7946,7 +7949,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8038,7 +8041,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8046,7 +8049,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8175,7 +8178,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8183,7 +8186,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8191,7 +8194,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8199,7 +8202,7 @@
         <v>60</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8218,7 +8221,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8240,7 +8243,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8251,7 +8254,7 @@
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8262,7 +8265,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8273,7 +8276,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8284,7 +8287,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8306,7 +8309,7 @@
         <v>21</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8317,7 +8320,7 @@
         <v>24</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8328,7 +8331,7 @@
         <v>27</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8339,7 +8342,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8350,7 +8353,7 @@
         <v>36</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8361,7 +8364,7 @@
         <v>40</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8369,7 +8372,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8377,7 +8380,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8385,7 +8388,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8393,7 +8396,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8409,7 +8412,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8417,7 +8420,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8425,7 +8428,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8433,7 +8436,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8441,7 +8444,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8449,7 +8452,7 @@
         <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8457,7 +8460,7 @@
         <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8473,7 +8476,7 @@
         <v>82</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8505,7 +8508,7 @@
         <v>82</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8513,7 +8516,7 @@
         <v>82</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8521,7 +8524,7 @@
         <v>82</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8529,7 +8532,7 @@
         <v>82</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8537,7 +8540,7 @@
         <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8569,7 +8572,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8577,7 +8580,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8593,7 +8596,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8601,7 +8604,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8617,7 +8620,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8633,7 +8636,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8649,7 +8652,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8657,7 +8660,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8665,7 +8668,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8689,7 +8692,7 @@
         <v>92</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8705,7 +8708,7 @@
         <v>92</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8713,7 +8716,7 @@
         <v>92</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8721,7 +8724,7 @@
         <v>92</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix clone saur tutor moves
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Trifox" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="295">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -2572,10 +2572,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3284,10 +3284,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3295,7 +3295,7 @@
         <v>92</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>99</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,7 +3303,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3311,7 +3311,7 @@
         <v>92</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,7 +3319,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3327,7 +3327,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3335,7 +3335,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3343,7 +3343,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,7 +3351,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3359,7 +3359,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3367,7 +3367,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3375,7 +3375,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3383,7 +3383,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3391,7 +3391,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>176</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3399,7 +3399,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3407,7 +3407,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3415,14 +3415,6 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C96" s="2" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3447,10 +3439,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4159,10 +4151,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4170,7 +4162,7 @@
         <v>92</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>99</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4178,7 +4170,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4186,7 +4178,7 @@
         <v>92</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,7 +4186,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4202,7 +4194,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4210,7 +4202,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4218,7 +4210,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4226,7 +4218,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4234,7 +4226,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4234,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4250,7 +4242,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4258,7 +4250,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4266,7 +4258,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>176</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,7 +4266,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,7 +4274,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4290,14 +4282,6 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C96" s="2" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4322,10 +4306,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5064,10 +5048,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5075,7 +5059,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>99</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,7 +5067,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,7 +5075,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5099,7 +5083,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5107,7 +5091,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5115,7 +5099,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5123,7 +5107,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5131,7 +5115,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5139,7 +5123,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5147,7 +5131,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,7 +5139,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5163,7 +5147,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5171,7 +5155,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>176</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,7 +5163,7 @@
         <v>92</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5187,7 +5171,7 @@
         <v>92</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5195,7 +5179,7 @@
         <v>92</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5203,7 +5187,7 @@
         <v>92</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,14 +5195,6 @@
         <v>92</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C101" s="2" t="s">
         <v>197</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix high jump kick
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Trifox" sheetId="1" state="visible" r:id="rId2"/>
@@ -1107,7 +1107,7 @@
     <t xml:space="preserve">Captivate</t>
   </si>
   <si>
-    <t xml:space="preserve">High Jump Kick</t>
+    <t xml:space="preserve">Hi Jump Kick</t>
   </si>
   <si>
     <t xml:space="preserve">Triple Kick</t>
@@ -11986,7 +11986,7 @@
   </sheetPr>
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
@@ -16360,8 +16360,8 @@
   </sheetPr>
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
more galarian ponyta stats
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3864" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3866" uniqueCount="556">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -1250,6 +1250,33 @@
     <t xml:space="preserve">UNICORN</t>
   </si>
   <si>
+    <t xml:space="preserve">EVO_LEVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This POKéMON will look into your eyes and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read the contents of your heart. If it finds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evil there, it promptly hides away. Its horn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hides a healing power.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heal Pulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healing Wish</t>
+  </si>
+  <si>
     <t xml:space="preserve">TURBAN</t>
   </si>
   <si>
@@ -1367,9 +1394,6 @@
     <t xml:space="preserve">CLONE_IVYSAUR</t>
   </si>
   <si>
-    <t xml:space="preserve">EVO_LEVEL</t>
-  </si>
-  <si>
     <t xml:space="preserve">An experimental POKéMON species created by</t>
   </si>
   <si>
@@ -1665,9 +1689,6 @@
   </si>
   <si>
     <t xml:space="preserve">slowly wear out the enemy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.0</t>
   </si>
   <si>
     <t xml:space="preserve">Blastoise</t>
@@ -5205,10 +5226,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5259,13 +5280,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>402</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5273,11 +5294,11 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>365</v>
+        <v>403</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5285,11 +5306,11 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>366</v>
+        <v>404</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5297,11 +5318,11 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>367</v>
+        <v>405</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5309,11 +5330,11 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>368</v>
+        <v>406</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5321,7 +5342,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5329,7 +5350,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>369</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5369,11 +5390,11 @@
         <v>26</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2" t="str">
         <f aca="false">CONCATENATE("total: ",SUM(B16:B21))</f>
-        <v>total: 200</v>
+        <v>total: 410</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5381,7 +5402,7 @@
         <v>27</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5389,7 +5410,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5397,7 +5418,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>30</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5405,7 +5426,7 @@
         <v>30</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>25</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5413,7 +5434,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5620,7 +5641,7 @@
         <v>63</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>65</v>
@@ -5631,7 +5652,7 @@
         <v>63</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>69</v>
@@ -5642,10 +5663,10 @@
         <v>63</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>67</v>
+        <v>392</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5653,7 +5674,7 @@
         <v>63</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>132</v>
@@ -5664,10 +5685,10 @@
         <v>63</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5675,10 +5696,10 @@
         <v>63</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5686,10 +5707,10 @@
         <v>63</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>374</v>
+        <v>408</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5697,10 +5718,10 @@
         <v>63</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>175</v>
+        <v>409</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5708,10 +5729,10 @@
         <v>63</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>67</v>
+        <v>393</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5719,10 +5740,10 @@
         <v>63</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>142</v>
+        <v>394</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5730,18 +5751,21 @@
         <v>63</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>393</v>
+        <v>410</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>60</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>376</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5749,7 +5773,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5757,7 +5781,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5765,7 +5789,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>84</v>
+        <v>378</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5773,7 +5797,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>379</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5781,7 +5805,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>77</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5789,7 +5813,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5797,7 +5821,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>376</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,7 +5829,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>140</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5813,7 +5837,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5821,7 +5845,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>380</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5829,7 +5853,7 @@
         <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5837,15 +5861,15 @@
         <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>83</v>
+        <v>382</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5853,7 +5877,7 @@
         <v>82</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5861,7 +5885,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5869,7 +5893,7 @@
         <v>82</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,7 +5901,7 @@
         <v>82</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5885,7 +5909,7 @@
         <v>82</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5893,7 +5917,7 @@
         <v>82</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5901,7 +5925,7 @@
         <v>82</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5909,15 +5933,15 @@
         <v>82</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5925,7 +5949,7 @@
         <v>92</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>98</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5933,7 +5957,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5941,7 +5965,7 @@
         <v>92</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5949,7 +5973,7 @@
         <v>92</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>94</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5957,7 +5981,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5965,7 +5989,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>219</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5973,7 +5997,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5981,7 +6005,7 @@
         <v>92</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5989,7 +6013,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5997,7 +6021,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>394</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6005,7 +6029,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6013,7 +6037,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>68</v>
+        <v>395</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6021,7 +6045,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>396</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6029,7 +6053,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6037,7 +6061,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6045,6 +6069,14 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>399</v>
       </c>
     </row>
@@ -6088,7 +6120,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6096,7 +6128,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6107,7 +6139,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6115,7 +6147,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6123,7 +6155,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C5" s="2" t="n">
         <f aca="false">LEN(B5)</f>
@@ -6136,7 +6168,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -6149,7 +6181,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -6162,7 +6194,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -6182,7 +6214,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6285,7 +6317,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6358,7 +6390,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6366,7 +6398,7 @@
         <v>45</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6406,7 +6438,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6414,7 +6446,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6422,7 +6454,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6430,7 +6462,7 @@
         <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6438,7 +6470,7 @@
         <v>60</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6457,7 +6489,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6479,7 +6511,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6501,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6523,7 +6555,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6556,7 +6588,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6567,7 +6599,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6578,7 +6610,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6589,7 +6621,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6600,7 +6632,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6611,7 +6643,7 @@
         <v>35</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6622,7 +6654,7 @@
         <v>40</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6633,7 +6665,7 @@
         <v>45</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6655,7 +6687,7 @@
         <v>55</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6666,7 +6698,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6677,7 +6709,7 @@
         <v>65</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6688,7 +6720,7 @@
         <v>70</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6824,7 +6856,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6856,7 +6888,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6979,7 +7011,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6987,7 +7019,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6998,7 +7030,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7006,7 +7038,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7014,10 +7046,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>441</v>
+        <v>402</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>16</v>
@@ -7028,7 +7060,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -7040,7 +7072,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -7052,7 +7084,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -7064,7 +7096,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -7273,7 +7305,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7305,7 +7337,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7313,7 +7345,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7321,7 +7353,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7337,7 +7369,7 @@
         <v>60</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7400,7 +7432,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7411,7 +7443,7 @@
         <v>11</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7422,7 +7454,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7523,7 +7555,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7539,7 +7571,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7795,7 +7827,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7846,7 +7878,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7854,7 +7886,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7865,7 +7897,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7873,7 +7905,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7881,10 +7913,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>441</v>
+        <v>402</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>36</v>
@@ -7895,7 +7927,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -7907,7 +7939,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -7919,7 +7951,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -7931,7 +7963,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -7951,7 +7983,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8140,7 +8172,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8172,7 +8204,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8180,7 +8212,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8188,7 +8220,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8204,7 +8236,7 @@
         <v>60</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8267,7 +8299,7 @@
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8278,7 +8310,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8289,7 +8321,7 @@
         <v>18</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8390,7 +8422,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8406,7 +8438,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8662,7 +8694,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8713,7 +8745,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8721,7 +8753,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8732,7 +8764,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8740,7 +8772,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8748,7 +8780,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="C5" s="2" t="n">
         <f aca="false">LEN(B5)</f>
@@ -8760,7 +8792,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -8772,7 +8804,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -8784,7 +8816,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -8804,7 +8836,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8993,7 +9025,7 @@
         <v>47</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9025,7 +9057,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9033,7 +9065,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9041,7 +9073,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9057,7 +9089,7 @@
         <v>60</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9109,7 +9141,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9131,7 +9163,7 @@
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9142,7 +9174,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9153,7 +9185,7 @@
         <v>18</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9263,7 +9295,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9287,7 +9319,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9303,7 +9335,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9559,7 +9591,7 @@
         <v>92</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9575,7 +9607,7 @@
         <v>92</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9583,7 +9615,7 @@
         <v>92</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -9626,7 +9658,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9634,7 +9666,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9645,7 +9677,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9653,7 +9685,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9661,10 +9693,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>441</v>
+        <v>402</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>16</v>
@@ -9675,7 +9707,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -9687,7 +9719,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -9699,7 +9731,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -9711,7 +9743,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -9731,7 +9763,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9920,7 +9952,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9952,7 +9984,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9960,7 +9992,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9968,7 +10000,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9976,7 +10008,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10080,7 +10112,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10102,7 +10134,7 @@
         <v>28</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10113,7 +10145,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10124,7 +10156,7 @@
         <v>36</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10135,7 +10167,7 @@
         <v>40</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10159,7 +10191,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10199,7 +10231,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10207,7 +10239,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10335,7 +10367,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10359,7 +10391,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10375,7 +10407,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10415,7 +10447,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10466,7 +10498,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10474,7 +10506,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10485,7 +10517,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10493,7 +10525,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10501,10 +10533,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>441</v>
+        <v>402</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>36</v>
@@ -10515,7 +10547,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -10527,7 +10559,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -10539,7 +10571,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -10551,7 +10583,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -10571,7 +10603,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10760,7 +10792,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10792,7 +10824,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10800,7 +10832,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10808,7 +10840,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10816,7 +10848,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10920,7 +10952,7 @@
         <v>24</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10942,7 +10974,7 @@
         <v>37</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10953,7 +10985,7 @@
         <v>42</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10964,7 +10996,7 @@
         <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10975,7 +11007,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10999,7 +11031,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11039,7 +11071,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11047,7 +11079,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11175,7 +11207,7 @@
         <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11199,7 +11231,7 @@
         <v>92</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11215,7 +11247,7 @@
         <v>92</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11255,7 +11287,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12036,7 +12068,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12044,7 +12076,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12055,7 +12087,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12063,7 +12095,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12071,7 +12103,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
       <c r="C5" s="2" t="n">
         <f aca="false">LEN(B5)</f>
@@ -12083,7 +12115,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -12095,7 +12127,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -12107,7 +12139,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -12127,7 +12159,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12227,7 +12259,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12316,7 +12348,7 @@
         <v>47</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12348,7 +12380,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12356,7 +12388,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12364,7 +12396,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12372,7 +12404,7 @@
         <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12476,7 +12508,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12498,7 +12530,7 @@
         <v>36</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12509,7 +12541,7 @@
         <v>39</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12520,7 +12552,7 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12531,7 +12563,7 @@
         <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12542,7 +12574,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12553,7 +12585,7 @@
         <v>60</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12564,7 +12596,7 @@
         <v>65</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12575,7 +12607,7 @@
         <v>70</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12599,7 +12631,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12639,7 +12671,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12647,7 +12679,7 @@
         <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12655,7 +12687,7 @@
         <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12783,7 +12815,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12807,7 +12839,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12823,7 +12855,7 @@
         <v>92</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12863,7 +12895,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12879,7 +12911,7 @@
         <v>92</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12895,7 +12927,7 @@
         <v>92</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -12938,7 +12970,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12946,7 +12978,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12957,7 +12989,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12965,7 +12997,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12973,10 +13005,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>441</v>
+        <v>402</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>16</v>
@@ -12987,7 +13019,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -12999,7 +13031,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -13011,7 +13043,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -13023,7 +13055,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -13043,7 +13075,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13232,7 +13264,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13264,7 +13296,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13272,7 +13304,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13280,7 +13312,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13288,7 +13320,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13337,7 +13369,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13348,7 +13380,7 @@
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13359,7 +13391,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13370,7 +13402,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13425,7 +13457,7 @@
         <v>27</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13436,7 +13468,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13458,7 +13490,7 @@
         <v>40</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13466,7 +13498,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13474,7 +13506,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13482,7 +13514,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13506,7 +13538,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13522,7 +13554,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13530,7 +13562,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13538,7 +13570,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13546,7 +13578,7 @@
         <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13554,7 +13586,7 @@
         <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13602,7 +13634,7 @@
         <v>82</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13618,7 +13650,7 @@
         <v>82</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13626,7 +13658,7 @@
         <v>82</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13634,7 +13666,7 @@
         <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13730,7 +13762,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13746,7 +13778,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13794,7 +13826,7 @@
         <v>92</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13861,7 +13893,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13869,7 +13901,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13880,7 +13912,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13888,7 +13920,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13896,10 +13928,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>441</v>
+        <v>402</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>36</v>
@@ -13910,7 +13942,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -13922,7 +13954,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -13934,7 +13966,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -13946,7 +13978,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">LEN(B9)</f>
@@ -13966,7 +13998,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>541</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14155,7 +14187,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14187,7 +14219,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14195,7 +14227,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14203,7 +14235,7 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14211,7 +14243,7 @@
         <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14260,7 +14292,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14271,7 +14303,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14282,7 +14314,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14293,7 +14325,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14348,7 +14380,7 @@
         <v>35</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14359,7 +14391,7 @@
         <v>41</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14381,7 +14413,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14389,7 +14421,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14397,7 +14429,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14405,7 +14437,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14429,7 +14461,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14445,7 +14477,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14453,7 +14485,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14461,7 +14493,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14469,7 +14501,7 @@
         <v>75</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14477,7 +14509,7 @@
         <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14525,7 +14557,7 @@
         <v>82</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14541,7 +14573,7 @@
         <v>82</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14549,7 +14581,7 @@
         <v>82</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14557,7 +14589,7 @@
         <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14653,7 +14685,7 @@
         <v>92</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14669,7 +14701,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14717,7 +14749,7 @@
         <v>92</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14784,7 +14816,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14792,7 +14824,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14803,7 +14835,7 @@
         <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14811,7 +14843,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14819,7 +14851,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="C5" s="2" t="n">
         <f aca="false">LEN(B5)</f>
@@ -14831,7 +14863,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">LEN(B6)</f>
@@ -14843,7 +14875,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">LEN(B7)</f>
@@ -14855,7 +14887,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">LEN(B8)</f>
@@ -14875,7 +14907,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14975,7 +15007,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15064,7 +15096,7 @@
         <v>47</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15096,7 +15128,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15104,7 +15136,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15112,7 +15144,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15120,7 +15152,7 @@
         <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15169,7 +15201,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15180,7 +15212,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15191,7 +15223,7 @@
         <v>9</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15202,7 +15234,7 @@
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15257,7 +15289,7 @@
         <v>35</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15268,7 +15300,7 @@
         <v>36</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15290,7 +15322,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15301,7 +15333,7 @@
         <v>50</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15312,7 +15344,7 @@
         <v>55</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15323,7 +15355,7 @@
         <v>60</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15334,7 +15366,7 @@
         <v>65</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15345,7 +15377,7 @@
         <v>70</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15353,7 +15385,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15361,7 +15393,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15369,7 +15401,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15393,7 +15425,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15409,7 +15441,7 @@
         <v>75</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15417,7 +15449,7 @@
         <v>75</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15425,7 +15457,7 @@
         <v>75</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15433,7 +15465,7 @@
         <v>75</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15441,7 +15473,7 @@
         <v>75</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15489,7 +15521,7 @@
         <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15505,7 +15537,7 @@
         <v>82</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15513,7 +15545,7 @@
         <v>82</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15521,7 +15553,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15617,7 +15649,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15633,7 +15665,7 @@
         <v>92</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15681,7 +15713,7 @@
         <v>92</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix galarian ponyta species identifier
</commit_message>
<xml_diff>
--- a/pokemon/new_species.xlsx
+++ b/pokemon/new_species.xlsx
@@ -5229,7 +5229,7 @@
   <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5245,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>